<commit_message>
Corrected excel sheets for application fix issues
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2386-MS-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-PREPAY-ON-15-JAN-DLR-Newcreateloan1.xlsx
+++ b/Mifos Automation Excels/Client/2386-MS-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-PREPAY-ON-15-JAN-DLR-Newcreateloan1.xlsx
@@ -321,15 +321,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -358,11 +355,6 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -685,138 +677,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>42005</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>42005</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>10000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>42005</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>10000</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>42005</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>42005</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -841,50 +833,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="17">
         <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="18">
         <v>42019</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="20">
         <v>3000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="21">
         <v>10015.34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -898,7 +890,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,80 +925,80 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="12">
         <v>10000</v>
       </c>
-      <c r="B2" s="14">
-        <v>9981.3700000000008</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11">
-        <v>18.63</v>
-      </c>
-      <c r="F2" s="11">
-        <v>18.63</v>
+      <c r="B2" s="12">
+        <v>10000</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
-        <v>34.19</v>
-      </c>
-      <c r="B3" s="11">
-        <v>33.97</v>
-      </c>
-      <c r="C3" s="11">
-        <v>0</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0</v>
-      </c>
-      <c r="E3" s="11">
-        <v>0.22</v>
-      </c>
-      <c r="F3" s="11">
-        <v>0.09</v>
+      <c r="A3" s="10">
+        <v>15.34</v>
+      </c>
+      <c r="B3" s="10">
+        <v>15.34</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>0</v>
-      </c>
-      <c r="B4" s="11">
-        <v>0</v>
-      </c>
-      <c r="C4" s="11">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="11">
-        <v>0</v>
-      </c>
-      <c r="F4" s="11">
+      <c r="A4" s="10">
+        <v>0</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
-        <v>0</v>
-      </c>
-      <c r="B5" s="11">
-        <v>0</v>
-      </c>
-      <c r="C5" s="11">
-        <v>0</v>
-      </c>
-      <c r="D5" s="11">
-        <v>0</v>
-      </c>
-      <c r="E5" s="11">
-        <v>0</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="A5" s="10">
+        <v>0</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1017,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD16"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,7 +1035,7 @@
     <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1093,104 +1085,77 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11">
         <v>42005</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="13">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="12">
         <v>10000</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11">
-        <v>0</v>
-      </c>
-      <c r="L2" s="11">
-        <v>0</v>
-      </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10">
+        <v>0</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0</v>
+      </c>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="P2" s="10"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>14</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>42019</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>42019</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="13">
+      <c r="E3" s="19"/>
+      <c r="F3" s="12">
         <v>10000</v>
       </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="18">
-        <f>G2*(4%/365)*B3</f>
-        <v>15.342465753424657</v>
-      </c>
-      <c r="I3" s="11">
-        <v>0</v>
-      </c>
-      <c r="J3" s="11">
-        <v>0</v>
-      </c>
-      <c r="K3" s="18">
-        <f>G2+H3</f>
-        <v>10015.342465753425</v>
-      </c>
-      <c r="L3" s="18">
-        <f>K3</f>
-        <v>10015.342465753425</v>
-      </c>
-      <c r="M3" s="11">
-        <v>0</v>
-      </c>
-      <c r="N3" s="11">
-        <v>0</v>
-      </c>
-      <c r="O3" s="11">
-        <v>0</v>
-      </c>
-      <c r="P3" s="11">
-        <v>0</v>
-      </c>
-      <c r="R3" s="20"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="18"/>
-      <c r="R4" s="20"/>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>15.34</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>10015.34</v>
+      </c>
+      <c r="L3" s="13">
+        <v>10015.34</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0</v>
+      </c>
+      <c r="P3" s="10">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1203,7 +1168,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,72 +1219,72 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
-        <v>29</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="10">
+        <v>19</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>42019</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="18">
-        <f>F2+G2</f>
-        <v>10015.342465753425</v>
-      </c>
-      <c r="F2" s="13">
+      <c r="E2" s="13">
+        <v>10015.34</v>
+      </c>
+      <c r="F2" s="12">
         <v>10000</v>
       </c>
-      <c r="G2" s="18">
-        <f>'Repayment schedule'!H3</f>
-        <v>15.342465753424657</v>
-      </c>
-      <c r="H2" s="11">
-        <v>0</v>
-      </c>
-      <c r="I2" s="11">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11">
-        <v>0</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="G2" s="10">
+        <v>15.34</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>42005</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>10000</v>
       </c>
-      <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="11">
-        <v>0</v>
-      </c>
-      <c r="J3" s="13">
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12">
         <v>10000</v>
       </c>
+      <c r="K3"/>
+      <c r="L3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1331,16 +1296,19 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B1" s="21">
         <v>10011.51</v>
       </c>
     </row>

</xml_diff>